<commit_message>
Fixed plot issues with last figure
</commit_message>
<xml_diff>
--- a/PolitoCliDyn_1stOrderCC/PolitoCliDyn_OutData/CDFitParameterTable_PartI.xlsx
+++ b/PolitoCliDyn_1stOrderCC/PolitoCliDyn_OutData/CDFitParameterTable_PartI.xlsx
@@ -287,7 +287,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.42645016728492791</v>
+        <v>0.42645016728492802</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -309,7 +309,7 @@
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0">
-        <v>0.002206301888816951</v>
+        <v>0.0022063018888169514</v>
       </c>
       <c r="H6" s="0"/>
     </row>
@@ -331,7 +331,7 @@
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0">
-        <v>4.856878041702978</v>
+        <v>4.8568780417029789</v>
       </c>
       <c r="H7" s="0"/>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.39906007975566793</v>
+        <v>0.39906007975566787</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -899,7 +899,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.44325170668777159</v>
+        <v>0.44325170668777164</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.35428990539606003</v>
+        <v>0.35428990539606009</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.35440918925704196</v>
+        <v>0.35440918925704207</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.53857157427290236</v>
+        <v>0.53857157427290225</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -3169,7 +3169,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.35542972020233993</v>
+        <v>0.35542972020233971</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -3191,7 +3191,7 @@
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0">
-        <v>0.0018621630537305595</v>
+        <v>0.0018621630537305582</v>
       </c>
       <c r="H6" s="0"/>
     </row>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0">
-        <v>4.1857533945912024</v>
+        <v>4.1857533945911989</v>
       </c>
       <c r="H7" s="0"/>
     </row>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.36244077923198731</v>
+        <v>0.36244077923198742</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -3497,7 +3497,7 @@
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0">
-        <v>0.0019313242727006994</v>
+        <v>0.0019313242727006996</v>
       </c>
       <c r="H6" s="0"/>
     </row>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0">
-        <v>3.9405776820101237</v>
+        <v>3.9405776820101241</v>
       </c>
       <c r="H7" s="0"/>
     </row>
@@ -3803,7 +3803,7 @@
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0">
-        <v>0.0020211813238448372</v>
+        <v>0.0020211813238448385</v>
       </c>
       <c r="H6" s="0"/>
     </row>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0">
-        <v>3.9503389004193266</v>
+        <v>3.9503389004193292</v>
       </c>
       <c r="H7" s="0"/>
     </row>
@@ -4087,7 +4087,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.38835573263843054</v>
+        <v>0.38835573263843048</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0">
-        <v>0.0020845278018444564</v>
+        <v>0.0020845278018444555</v>
       </c>
       <c r="H6" s="0"/>
     </row>
@@ -4131,7 +4131,7 @@
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0">
-        <v>4.1142817759327093</v>
+        <v>4.1142817759327075</v>
       </c>
       <c r="H7" s="0"/>
     </row>
@@ -4699,7 +4699,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.39931905658139916</v>
+        <v>0.39931905658139927</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0">
-        <v>0.0021179761440220167</v>
+        <v>0.0021179761440220171</v>
       </c>
       <c r="H6" s="0"/>
     </row>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0">
-        <v>4.3381330678252219</v>
+        <v>4.3381330678252228</v>
       </c>
       <c r="H7" s="0"/>
     </row>
@@ -5005,7 +5005,7 @@
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0">
-        <v>0.39383424967537795</v>
+        <v>0.393834249675378</v>
       </c>
       <c r="H5" s="0"/>
     </row>
@@ -5027,7 +5027,7 @@
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0">
-        <v>0.0020797248511480121</v>
+        <v>0.0020797248511480126</v>
       </c>
       <c r="H6" s="0"/>
     </row>
@@ -5049,7 +5049,7 @@
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0">
-        <v>4.3032955270974309</v>
+        <v>4.3032955270974318</v>
       </c>
       <c r="H7" s="0"/>
     </row>

</xml_diff>